<commit_message>
updated NOR FIN AND MLS
</commit_message>
<xml_diff>
--- a/FIN.xlsx
+++ b/FIN.xlsx
@@ -2523,10 +2523,10 @@
   <dimension ref="A1:BQ133"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AP56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AP35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A62" sqref="A62:XFD62"/>
+      <selection pane="bottomRight" activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35263,7 +35263,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" activeCellId="1" sqref="A11:XFD11 A4:XFD4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>